<commit_message>
Zwischenstand: aw_wahl und aw_wahlperiode
</commit_message>
<xml_diff>
--- a/daten/tabelle-direktkandidaten-aw.xlsx
+++ b/daten/tabelle-direktkandidaten-aw.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="861">
   <si>
     <t xml:space="preserve">wk</t>
   </si>
@@ -2357,12 +2357,18 @@
     <t xml:space="preserve">Stachowiak</t>
   </si>
   <si>
-    <t xml:space="preserve">1993</t>
+    <t xml:space="preserve">Pilgram</t>
   </si>
   <si>
     <t xml:space="preserve">Elektroingenieur (B.Sc.)</t>
   </si>
   <si>
+    <t xml:space="preserve">Reinheim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Kleingewerbe selbstständig im Bereich PC-Service</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.abgeordnetenwatch.de/profile/dieter-stein</t>
   </si>
   <si>
@@ -2495,6 +2501,15 @@
     <t xml:space="preserve">Ermen</t>
   </si>
   <si>
+    <t xml:space="preserve">Diplom-Informatikerin (RWTH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bensheim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketing-Beraterin für Heilpraktiker</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.abgeordnetenwatch.de/profile/kerstin-buchner</t>
   </si>
   <si>
@@ -2550,9 +2565,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ethnologe,  Politikwissenschaftler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bensheim</t>
   </si>
   <si>
     <t xml:space="preserve">Doktorand</t>
@@ -6080,7 +6092,7 @@
         <v>341</v>
       </c>
       <c r="Q72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R72"/>
     </row>
@@ -7090,7 +7102,9 @@
       <c r="Q94" t="n">
         <v>2</v>
       </c>
-      <c r="R94"/>
+      <c r="R94" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -7569,8 +7583,12 @@
       <c r="J105" t="s">
         <v>492</v>
       </c>
-      <c r="K105"/>
-      <c r="L105"/>
+      <c r="K105" t="s">
+        <v>492</v>
+      </c>
+      <c r="L105" t="s">
+        <v>29</v>
+      </c>
       <c r="M105" t="n">
         <v>1983</v>
       </c>
@@ -7814,7 +7832,7 @@
         <v>516</v>
       </c>
       <c r="Q110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R110"/>
     </row>
@@ -8271,7 +8289,7 @@
         <v>2</v>
       </c>
       <c r="R120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
@@ -8530,7 +8548,7 @@
         <v>98</v>
       </c>
       <c r="Q126" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R126" t="n">
         <v>31</v>
@@ -8748,7 +8766,9 @@
       <c r="Q131" t="n">
         <v>2</v>
       </c>
-      <c r="R131"/>
+      <c r="R131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -10138,7 +10158,7 @@
         <v>98</v>
       </c>
       <c r="Q162" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R162" t="n">
         <v>2</v>
@@ -10768,13 +10788,21 @@
       <c r="K176" t="s">
         <v>781</v>
       </c>
-      <c r="L176"/>
-      <c r="M176"/>
+      <c r="L176" t="s">
+        <v>41</v>
+      </c>
+      <c r="M176" t="n">
+        <v>1993</v>
+      </c>
       <c r="N176" t="s">
         <v>782</v>
       </c>
-      <c r="O176"/>
-      <c r="P176"/>
+      <c r="O176" t="s">
+        <v>783</v>
+      </c>
+      <c r="P176" t="s">
+        <v>784</v>
+      </c>
       <c r="Q176"/>
       <c r="R176"/>
     </row>
@@ -10789,7 +10817,7 @@
         <v>176840</v>
       </c>
       <c r="D177" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E177" t="n">
         <v>15</v>
@@ -10803,7 +10831,7 @@
         <v>645</v>
       </c>
       <c r="J177" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="K177"/>
       <c r="L177"/>
@@ -10827,7 +10855,7 @@
         <v>176414</v>
       </c>
       <c r="D178" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="E178" t="n">
         <v>193</v>
@@ -10838,13 +10866,13 @@
       <c r="G178"/>
       <c r="H178"/>
       <c r="I178" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="J178" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="K178" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="L178" t="s">
         <v>29</v>
@@ -10853,13 +10881,13 @@
         <v>1990</v>
       </c>
       <c r="N178" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="O178" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="P178" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="Q178"/>
       <c r="R178"/>
@@ -10875,7 +10903,7 @@
         <v>176377</v>
       </c>
       <c r="D179" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="E179" t="n">
         <v>201</v>
@@ -10886,10 +10914,10 @@
       <c r="G179"/>
       <c r="H179"/>
       <c r="I179" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="J179" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="K179"/>
       <c r="L179" t="s">
@@ -10899,13 +10927,13 @@
         <v>1950</v>
       </c>
       <c r="N179" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="O179" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="P179" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="Q179"/>
       <c r="R179"/>
@@ -10921,7 +10949,7 @@
         <v>159624</v>
       </c>
       <c r="D180" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="E180" t="n">
         <v>7</v>
@@ -10932,7 +10960,7 @@
       <c r="G180"/>
       <c r="H180"/>
       <c r="I180" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="J180" t="s">
         <v>266</v>
@@ -10945,11 +10973,11 @@
         <v>1994</v>
       </c>
       <c r="N180" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="O180"/>
       <c r="P180" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="Q180"/>
       <c r="R180"/>
@@ -10965,7 +10993,7 @@
         <v>79150</v>
       </c>
       <c r="D181" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="E181" t="n">
         <v>2</v>
@@ -10976,10 +11004,10 @@
       <c r="G181"/>
       <c r="H181"/>
       <c r="I181" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="J181" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="K181"/>
       <c r="L181" t="s">
@@ -10989,16 +11017,16 @@
         <v>1963</v>
       </c>
       <c r="N181" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="O181" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="P181" t="s">
         <v>98</v>
       </c>
       <c r="Q181" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R181" t="n">
         <v>19</v>
@@ -11015,7 +11043,7 @@
         <v>175776</v>
       </c>
       <c r="D182" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="E182" t="n">
         <v>4</v>
@@ -11026,10 +11054,10 @@
       <c r="G182"/>
       <c r="H182"/>
       <c r="I182" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="J182" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="K182"/>
       <c r="L182" t="s">
@@ -11040,10 +11068,10 @@
       </c>
       <c r="N182"/>
       <c r="O182" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="P182" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="Q182" t="n">
         <v>1</v>
@@ -11063,7 +11091,7 @@
         <v>159644</v>
       </c>
       <c r="D183" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="E183" t="n">
         <v>5</v>
@@ -11076,10 +11104,10 @@
       </c>
       <c r="H183"/>
       <c r="I183" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="J183" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="K183"/>
       <c r="L183" t="s">
@@ -11091,7 +11119,7 @@
       <c r="N183"/>
       <c r="O183"/>
       <c r="P183" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="Q183"/>
       <c r="R183"/>
@@ -11107,7 +11135,7 @@
         <v>175345</v>
       </c>
       <c r="D184" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="E184" t="n">
         <v>8</v>
@@ -11120,10 +11148,10 @@
       </c>
       <c r="H184"/>
       <c r="I184" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="J184" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="K184"/>
       <c r="L184" t="s">
@@ -11134,10 +11162,10 @@
       </c>
       <c r="N184"/>
       <c r="O184" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="P184" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="Q184"/>
       <c r="R184"/>
@@ -11153,7 +11181,7 @@
         <v>78792</v>
       </c>
       <c r="D185" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="E185" t="n">
         <v>1</v>
@@ -11177,7 +11205,7 @@
         <v>1981</v>
       </c>
       <c r="N185" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="O185"/>
       <c r="P185" t="s">
@@ -11195,34 +11223,44 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C186" t="n">
         <v>177265</v>
       </c>
       <c r="D186" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="E186" t="n">
         <v>149</v>
       </c>
       <c r="F186" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="G186"/>
       <c r="H186"/>
       <c r="I186" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="J186" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="K186"/>
-      <c r="L186"/>
-      <c r="M186"/>
-      <c r="N186"/>
-      <c r="O186"/>
-      <c r="P186"/>
+      <c r="L186" t="s">
+        <v>29</v>
+      </c>
+      <c r="M186" t="n">
+        <v>1967</v>
+      </c>
+      <c r="N186" t="s">
+        <v>829</v>
+      </c>
+      <c r="O186" t="s">
+        <v>830</v>
+      </c>
+      <c r="P186" t="s">
+        <v>831</v>
+      </c>
       <c r="Q186"/>
       <c r="R186"/>
     </row>
@@ -11231,13 +11269,13 @@
         <v>188</v>
       </c>
       <c r="B187" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C187" t="n">
         <v>165416</v>
       </c>
       <c r="D187" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="E187" t="n">
         <v>7</v>
@@ -11250,10 +11288,10 @@
       </c>
       <c r="H187"/>
       <c r="I187" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="J187" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="K187"/>
       <c r="L187" t="s">
@@ -11263,13 +11301,13 @@
         <v>1965</v>
       </c>
       <c r="N187" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O187" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="P187" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="Q187"/>
       <c r="R187"/>
@@ -11279,13 +11317,13 @@
         <v>188</v>
       </c>
       <c r="B188" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C188" t="n">
         <v>165416</v>
       </c>
       <c r="D188" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="E188" t="n">
         <v>7</v>
@@ -11298,10 +11336,10 @@
       </c>
       <c r="H188"/>
       <c r="I188" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="J188" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="K188"/>
       <c r="L188" t="s">
@@ -11311,13 +11349,13 @@
         <v>1965</v>
       </c>
       <c r="N188" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O188" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="P188" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="Q188"/>
       <c r="R188"/>
@@ -11327,13 +11365,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C189" t="n">
         <v>176136</v>
       </c>
       <c r="D189" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="E189" t="n">
         <v>201</v>
@@ -11344,10 +11382,10 @@
       <c r="G189"/>
       <c r="H189"/>
       <c r="I189" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="J189" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="K189"/>
       <c r="L189"/>
@@ -11363,13 +11401,13 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C190" t="n">
         <v>165416</v>
       </c>
       <c r="D190" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="E190" t="n">
         <v>7</v>
@@ -11380,10 +11418,10 @@
       <c r="G190"/>
       <c r="H190"/>
       <c r="I190" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="J190" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="K190"/>
       <c r="L190" t="s">
@@ -11393,13 +11431,13 @@
         <v>1965</v>
       </c>
       <c r="N190" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O190" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="P190" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="Q190"/>
       <c r="R190"/>
@@ -11409,13 +11447,13 @@
         <v>188</v>
       </c>
       <c r="B191" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C191" t="n">
         <v>165416</v>
       </c>
       <c r="D191" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="E191" t="n">
         <v>7</v>
@@ -11426,10 +11464,10 @@
       <c r="G191"/>
       <c r="H191"/>
       <c r="I191" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="J191" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="K191"/>
       <c r="L191" t="s">
@@ -11439,13 +11477,13 @@
         <v>1965</v>
       </c>
       <c r="N191" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O191" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="P191" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="Q191"/>
       <c r="R191"/>
@@ -11455,13 +11493,13 @@
         <v>188</v>
       </c>
       <c r="B192" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C192" t="n">
         <v>79135</v>
       </c>
       <c r="D192" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="E192" t="n">
         <v>2</v>
@@ -11475,7 +11513,7 @@
         <v>70</v>
       </c>
       <c r="J192" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="K192"/>
       <c r="L192" t="s">
@@ -11485,7 +11523,7 @@
         <v>1961</v>
       </c>
       <c r="N192" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="O192"/>
       <c r="P192" t="s">
@@ -11501,13 +11539,13 @@
         <v>188</v>
       </c>
       <c r="B193" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C193" t="n">
         <v>122050</v>
       </c>
       <c r="D193" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="E193" t="n">
         <v>4</v>
@@ -11518,10 +11556,10 @@
       <c r="G193"/>
       <c r="H193"/>
       <c r="I193" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="J193" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="K193"/>
       <c r="L193" t="s">
@@ -11531,7 +11569,7 @@
         <v>1968</v>
       </c>
       <c r="N193" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="O193"/>
       <c r="P193" t="s">
@@ -11549,13 +11587,13 @@
         <v>188</v>
       </c>
       <c r="B194" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C194" t="n">
         <v>145995</v>
       </c>
       <c r="D194" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="E194" t="n">
         <v>5</v>
@@ -11568,7 +11606,7 @@
       </c>
       <c r="H194"/>
       <c r="I194" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="J194" t="s">
         <v>359</v>
@@ -11581,13 +11619,13 @@
         <v>1992</v>
       </c>
       <c r="N194" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="O194" t="s">
-        <v>846</v>
+        <v>830</v>
       </c>
       <c r="P194" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="Q194"/>
       <c r="R194"/>
@@ -11597,13 +11635,13 @@
         <v>188</v>
       </c>
       <c r="B195" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C195" t="n">
         <v>175499</v>
       </c>
       <c r="D195" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="E195" t="n">
         <v>1</v>
@@ -11614,10 +11652,10 @@
       <c r="G195"/>
       <c r="H195"/>
       <c r="I195" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="J195" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="K195"/>
       <c r="L195" t="s">
@@ -11627,11 +11665,11 @@
         <v>1980</v>
       </c>
       <c r="N195" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="O195"/>
       <c r="P195" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="Q195"/>
       <c r="R195"/>
@@ -11641,13 +11679,13 @@
         <v>188</v>
       </c>
       <c r="B196" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C196" t="n">
         <v>146138</v>
       </c>
       <c r="D196" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="E196" t="n">
         <v>8</v>
@@ -11658,10 +11696,10 @@
       <c r="G196"/>
       <c r="H196"/>
       <c r="I196" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="J196" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="K196"/>
       <c r="L196" t="s">
@@ -11675,7 +11713,7 @@
       </c>
       <c r="O196"/>
       <c r="P196" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="Q196"/>
       <c r="R196"/>

</xml_diff>